<commit_message>
Edits all .xlsx files in directory
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\TimeSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43DD3BC-6A2E-46A5-99DB-7C879D77724A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0022C28-4680-4942-8067-EB6220679375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1930" windowWidth="13330" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="3" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <t>Day</t>
   </si>
   <si>
-    <t>April</t>
-  </si>
-  <si>
     <t>MON TUE WED THU FRI SAT</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t xml:space="preserve">DIA CODE: </t>
+  </si>
+  <si>
+    <t>May</t>
   </si>
 </sst>
 </file>
@@ -427,10 +427,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -810,7 +810,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -822,7 +822,7 @@
     </row>
     <row r="2" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -844,25 +844,25 @@
     </row>
     <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
       <c r="D4" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="39" t="s">
         <v>22</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>23</v>
       </c>
       <c r="F4" s="39"/>
       <c r="G4" s="38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="38"/>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="40"/>
       <c r="C5" s="40"/>
@@ -874,15 +874,15 @@
     </row>
     <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="35"/>
       <c r="C6" s="35"/>
       <c r="D6" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
@@ -890,14 +890,14 @@
     </row>
     <row r="7" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="40"/>
       <c r="C7" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
@@ -910,14 +910,14 @@
       </c>
       <c r="B8" s="36"/>
       <c r="C8" s="35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="36"/>
       <c r="E8" s="30" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G8" s="37"/>
       <c r="H8" s="12">
@@ -984,11 +984,11 @@
     </row>
     <row r="12" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="str" cm="1">
-        <f t="array" ref="A12:B37">_xlfn._xlws.FILTER(IF(Draft!$A$12:'Draft'!$B$40&lt;&gt;0, Draft!$A$12:'Draft'!$B$40, ""), (ROW(Draft!$A$12:'Draft'!$A$40) &lt;= MAX(_xlfn._xlws.FILTER(ROW(Draft!$A$12:'Draft'!$A$40), Draft!$A$12:'Draft'!$A$40&lt;&gt;""))))</f>
-        <v>星期一</v>
+        <f t="array" ref="A12:B38">_xlfn._xlws.FILTER(IF(Draft!$A$12:'Draft'!$B$40&lt;&gt;0, Draft!$A$12:'Draft'!$B$40, ""), (ROW(Draft!$A$12:'Draft'!$A$40) &lt;= MAX(_xlfn._xlws.FILTER(ROW(Draft!$A$12:'Draft'!$A$40), Draft!$A$12:'Draft'!$A$40&lt;&gt;""))))</f>
+        <v>星期三</v>
       </c>
       <c r="B12" s="11">
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -999,194 +999,194 @@
     </row>
     <row r="13" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="B13" s="11">
-        <v>45384</v>
+        <v>45414</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="B14" s="11">
-        <v>45385</v>
+        <v>45415</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="B15" s="11">
-        <v>45386</v>
+        <v>45416</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="B16" s="11">
-        <v>45387</v>
+        <v>45418</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="B17" s="11">
-        <v>45388</v>
+        <v>45419</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="B18" s="11">
-        <v>45390</v>
+        <v>45420</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="B19" s="11">
-        <v>45391</v>
+        <v>45421</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="B20" s="11">
-        <v>45392</v>
+        <v>45422</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="B21" s="11">
-        <v>45393</v>
+        <v>45423</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="B22" s="11">
-        <v>45394</v>
+        <v>45425</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="14" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="B23" s="11">
-        <v>45395</v>
+        <v>45426</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="14" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="B24" s="11">
-        <v>45397</v>
+        <v>45427</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="B25" s="11">
-        <v>45398</v>
+        <v>45428</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="B26" s="11">
-        <v>45399</v>
+        <v>45429</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="B27" s="11">
-        <v>45400</v>
+        <v>45430</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="B28" s="11">
-        <v>45401</v>
+        <v>45432</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="14" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="B29" s="11">
-        <v>45402</v>
+        <v>45433</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="B30" s="11">
-        <v>45404</v>
+        <v>45434</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="31" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="B31" s="28">
-        <v>45405</v>
+        <v>45435</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="31" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="B32" s="28">
-        <v>45406</v>
+        <v>45436</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="31" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="B33" s="28">
-        <v>45407</v>
+        <v>45437</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="28" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="B34" s="32">
-        <v>45408</v>
+        <v>45439</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="31" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="B35" s="28">
-        <v>45409</v>
+        <v>45440</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="31" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="B36" s="28">
-        <v>45411</v>
+        <v>45441</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1197,10 +1197,10 @@
     </row>
     <row r="37" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="31" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="B37" s="28">
-        <v>45412</v>
+        <v>45442</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1210,8 +1210,12 @@
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="31"/>
-      <c r="B38" s="28"/>
+      <c r="A38" s="31" t="str">
+        <v>星期五</v>
+      </c>
+      <c r="B38" s="28">
+        <v>45443</v>
+      </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -4072,7 +4076,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="41" t="str">
+      <c r="A1" s="42" t="str">
         <f>Final!$A$1</f>
         <v>VERY GOOD COMPANY INC</v>
       </c>
@@ -4085,7 +4089,7 @@
       <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="41" t="str">
+      <c r="A2" s="42" t="str">
         <f>Final!$A$2</f>
         <v>PARTICIPANT SIGN IN SHEET</v>
       </c>
@@ -4186,11 +4190,11 @@
         <f>Final!$E$8</f>
         <v>MONTH:</v>
       </c>
-      <c r="F8" s="42" t="str">
+      <c r="F8" s="41" t="str">
         <f>Final!$F$8</f>
-        <v>April</v>
-      </c>
-      <c r="G8" s="42"/>
+        <v>May</v>
+      </c>
+      <c r="G8" s="41"/>
       <c r="H8" s="12">
         <f>Final!$H$8</f>
         <v>2024</v>
@@ -4256,12 +4260,12 @@
     </row>
     <row r="12" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="str" cm="1">
-        <f t="array" ref="A12:A37">_xlfn._xlws.FILTER(Formulas!$K$1:'Formulas'!$K$31,Formulas!$K$1:'Formulas'!$K$31&lt;&gt;"")</f>
-        <v>星期一</v>
+        <f t="array" ref="A12:A38">_xlfn._xlws.FILTER(Formulas!$K$1:'Formulas'!$K$31,Formulas!$K$1:'Formulas'!$K$31&lt;&gt;"")</f>
+        <v>星期三</v>
       </c>
       <c r="B12" s="11" cm="1">
-        <f t="array" ref="B12:B37">_xlfn._xlws.FILTER(Formulas!$J$1:'Formulas'!$J$31,Formulas!$J$1:'Formulas'!$J$31&lt;&gt;"")</f>
-        <v>45383</v>
+        <f t="array" ref="B12:B38">_xlfn._xlws.FILTER(Formulas!$J$1:'Formulas'!$J$31,Formulas!$J$1:'Formulas'!$J$31&lt;&gt;"")</f>
+        <v>45413</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -4272,194 +4276,194 @@
     </row>
     <row r="13" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="B13" s="11">
-        <v>45384</v>
+        <v>45414</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="B14" s="11">
-        <v>45385</v>
+        <v>45415</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="B15" s="11">
-        <v>45386</v>
+        <v>45416</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="B16" s="11">
-        <v>45387</v>
+        <v>45418</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="B17" s="11">
-        <v>45388</v>
+        <v>45419</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="B18" s="11">
-        <v>45390</v>
+        <v>45420</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="B19" s="11">
-        <v>45391</v>
+        <v>45421</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="B20" s="11">
-        <v>45392</v>
+        <v>45422</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="B21" s="11">
-        <v>45393</v>
+        <v>45423</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="B22" s="11">
-        <v>45394</v>
+        <v>45425</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="14" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="B23" s="11">
-        <v>45395</v>
+        <v>45426</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="14" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="B24" s="11">
-        <v>45397</v>
+        <v>45427</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="B25" s="11">
-        <v>45398</v>
+        <v>45428</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="B26" s="11">
-        <v>45399</v>
+        <v>45429</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="B27" s="11">
-        <v>45400</v>
+        <v>45430</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="B28" s="11">
-        <v>45401</v>
+        <v>45432</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="29" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="B29" s="11">
-        <v>45402</v>
+        <v>45433</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="29" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="B30" s="11">
-        <v>45404</v>
+        <v>45434</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="B31" s="28">
-        <v>45405</v>
+        <v>45435</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="B32" s="28">
-        <v>45406</v>
+        <v>45436</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="B33" s="28">
-        <v>45407</v>
+        <v>45437</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="B34" s="28">
-        <v>45408</v>
+        <v>45439</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="B35" s="22">
-        <v>45409</v>
+        <v>45440</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="B36" s="22">
-        <v>45411</v>
+        <v>45441</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -4470,10 +4474,10 @@
     </row>
     <row r="37" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="B37" s="22">
-        <v>45412</v>
+        <v>45442</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -4483,7 +4487,12 @@
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="22"/>
+      <c r="A38" t="str">
+        <v>星期五</v>
+      </c>
+      <c r="B38" s="22">
+        <v>45443</v>
+      </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -7283,6 +7292,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="E6:H6"/>
@@ -7290,12 +7305,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <conditionalFormatting sqref="A12:B40">
     <cfRule type="expression" dxfId="4" priority="1">
@@ -7334,7 +7343,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="41" t="str">
+      <c r="A1" s="42" t="str">
         <f>Final!$A$1</f>
         <v>VERY GOOD COMPANY INC</v>
       </c>
@@ -7347,7 +7356,7 @@
       <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="41" t="str">
+      <c r="A2" s="42" t="str">
         <f>Final!$A$2</f>
         <v>PARTICIPANT SIGN IN SHEET</v>
       </c>
@@ -7448,11 +7457,11 @@
         <f>Final!$E$8</f>
         <v>MONTH:</v>
       </c>
-      <c r="F8" s="42" t="str">
+      <c r="F8" s="41" t="str">
         <f>Final!$F$8</f>
-        <v>April</v>
-      </c>
-      <c r="G8" s="42"/>
+        <v>May</v>
+      </c>
+      <c r="G8" s="41"/>
       <c r="H8" s="12">
         <f>Final!$H$8</f>
         <v>2024</v>
@@ -7519,11 +7528,11 @@
     <row r="12" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="str" cm="1">
         <f t="array" ref="A12:A29">_xlfn._xlws.FILTER(Formulas!$K$1:'Formulas'!$K$18, (ROW(Formulas!$K$1:'Formulas'!$K$18)&lt;19)*(Formulas!$K$1:'Formulas'!$K$18&lt;&gt;""))</f>
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="B12" s="11" cm="1">
         <f t="array" ref="B12:B29">_xlfn._xlws.FILTER(Formulas!$J$1:'Formulas'!$J$18, (ROW(Formulas!$J$1:'Formulas'!$J$18)&lt;19)*(Formulas!$J$1:'Formulas'!$J$18&lt;&gt;""))</f>
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -7534,196 +7543,196 @@
     </row>
     <row r="13" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="B13" s="11">
-        <v>45384</v>
+        <v>45414</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="B14" s="11">
-        <v>45385</v>
+        <v>45415</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="B15" s="11">
-        <v>45386</v>
+        <v>45416</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="B16" s="11">
-        <v>45387</v>
+        <v>45418</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="B17" s="11">
-        <v>45388</v>
+        <v>45419</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="B18" s="11">
-        <v>45390</v>
+        <v>45420</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="B19" s="11">
-        <v>45391</v>
+        <v>45421</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="B20" s="11">
-        <v>45392</v>
+        <v>45422</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="B21" s="11">
-        <v>45393</v>
+        <v>45423</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="B22" s="11">
-        <v>45394</v>
+        <v>45425</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="14" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="B23" s="11">
-        <v>45395</v>
+        <v>45426</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="14" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="B24" s="11">
-        <v>45397</v>
+        <v>45427</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="B25" s="11">
-        <v>45398</v>
+        <v>45428</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="B26" s="11">
-        <v>45399</v>
+        <v>45429</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="B27" s="11">
-        <v>45400</v>
+        <v>45430</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="B28" s="11">
-        <v>45401</v>
+        <v>45432</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="29" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="B29" s="11">
-        <v>45402</v>
+        <v>45433</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="29" t="str" cm="1">
-        <f t="array" ref="A30:A37">IFERROR(_xlfn._xlws.FILTER(Formulas!$K$20:'Formulas'!$K$31, (ROW(Formulas!$K$20:'Formulas'!$K$31)&gt;19)*(Formulas!$K$20:'Formulas'!$K$31&lt;&gt;"")), "")</f>
-        <v>星期一</v>
+        <f t="array" ref="A30:A38">IFERROR(_xlfn._xlws.FILTER(Formulas!$K$20:'Formulas'!$K$31, (ROW(Formulas!$K$20:'Formulas'!$K$31)&gt;19)*(Formulas!$K$20:'Formulas'!$K$31&lt;&gt;"")), "")</f>
+        <v>星期三</v>
       </c>
       <c r="B30" s="11" cm="1">
-        <f t="array" ref="B30:B37">IFERROR(_xlfn._xlws.FILTER(Formulas!$J$20:'Formulas'!$J$31, (ROW(Formulas!$J$20:'Formulas'!$J$31)&gt;19)*(Formulas!$J$20:'Formulas'!$J$31&lt;&gt;"")), "")</f>
-        <v>45404</v>
+        <f t="array" ref="B30:B38">IFERROR(_xlfn._xlws.FILTER(Formulas!$J$20:'Formulas'!$J$31, (ROW(Formulas!$J$20:'Formulas'!$J$31)&gt;19)*(Formulas!$J$20:'Formulas'!$J$31&lt;&gt;"")), "")</f>
+        <v>45434</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="B31" s="28">
-        <v>45405</v>
+        <v>45435</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="B32" s="28">
-        <v>45406</v>
+        <v>45436</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="B33" s="28">
-        <v>45407</v>
+        <v>45437</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="B34" s="28">
-        <v>45408</v>
+        <v>45439</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="B35" s="22">
-        <v>45409</v>
+        <v>45440</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="B36" s="22">
-        <v>45411</v>
+        <v>45441</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -7734,10 +7743,10 @@
     </row>
     <row r="37" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="B37" s="22">
-        <v>45412</v>
+        <v>45442</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -7747,7 +7756,12 @@
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="22"/>
+      <c r="A38" t="str">
+        <v>星期五</v>
+      </c>
+      <c r="B38" s="22">
+        <v>45443</v>
+      </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -10607,37 +10621,37 @@
     <row r="1" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="13">
         <f>DATEVALUE(Draft!$F$8 &amp; " 1, " &amp; Draft!$H$8)</f>
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="C1" s="4" cm="1">
-        <f t="array" ref="C1:C30">_xlfn.SEQUENCE(DAY(EOMONTH(A1,0)), 1,A1, 1)</f>
-        <v>45383</v>
+        <f t="array" ref="C1:C31">_xlfn.SEQUENCE(DAY(EOMONTH(A1,0)), 1,A1, 1)</f>
+        <v>45413</v>
       </c>
       <c r="D1" s="5">
         <f>IF($C1="","",WEEKDAY($C1)-1)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="4" cm="1">
-        <f t="array" ref="F1:F26">_xlfn._xlws.FILTER($C$1:$C$31, ($D$1:$D$31=$N$1)+($D$1:$D$31=$N$2)+($D$1:$D$31=$N$3)+($D$1:$D$31=$N$4)+($D$1:$D$31=$N$5)+($D$1:$D$31=$N$6), "")</f>
-        <v>45383</v>
+        <f t="array" ref="F1:F27">_xlfn._xlws.FILTER($C$1:$C$31, ($D$1:$D$31=$N$1)+($D$1:$D$31=$N$2)+($D$1:$D$31=$N$3)+($D$1:$D$31=$N$4)+($D$1:$D$31=$N$5)+($D$1:$D$31=$N$6), "")</f>
+        <v>45413</v>
       </c>
       <c r="G1" s="5">
         <f>IF($F1="","",WEEKDAY($F1)-1)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H1" s="5" t="str">
         <f t="shared" ref="H1:H31" si="0">IF($G1=1, "星期一", IF($G1=2, "星期二", IF($G1=3, "星期三", IF($G1=4, "星期四", IF($G1=5, "星期五", IF($G1=6, "星期六", ""))))))</f>
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="I1" s="6"/>
       <c r="J1" s="18" cm="1">
         <f t="array" ref="J1:J18">IF(OR(ISBLANK($F$19), $F$24&lt;&gt;""), _xlfn._xlws.FILTER($F$1:$F$31, (ROW($F$1:$F$31)&lt;19)*($F$1:$F$31&lt;&gt;"")), _xlfn._xlws.FILTER($F$1:$F$31, (ROW($F$1:$F$31)&lt;=COUNT($F$1:$F$31)-5)*($F$1:$F$31&lt;&gt;"")))</f>
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="K1" s="16" t="str" cm="1">
         <f t="array" ref="K1:K18">IF(OR(ISBLANK($F$19), $F$24&lt;&gt;""), _xlfn._xlws.FILTER($H$1:$H$31, (ROW($F$1:$F$31)&lt;19)*($F$1:$F$31&lt;&gt;"")), _xlfn._xlws.FILTER($H$1:$H$31, (ROW($F$1:$F$31)&lt;=COUNT($F$1:$F$31)-5)*($F$1:$F$31&lt;&gt;"")))</f>
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="L1" s="6"/>
       <c r="M1" s="5" t="str" cm="1">
@@ -10650,39 +10664,39 @@
       </c>
       <c r="P1" s="25" t="str" cm="1">
         <f t="array" ref="P1:P18">_xlfn._xlws.FILTER(Formulas!$K$1:'Formulas'!$K$18, (ROW(Formulas!$K$1:'Formulas'!$K$18)&lt;19)*(Formulas!$K$1:'Formulas'!$K$18&lt;&gt;""))</f>
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="Q1" s="26" cm="1">
         <f t="array" ref="Q1:Q18">_xlfn._xlws.FILTER(Formulas!$J$1:'Formulas'!$J$18, (ROW(Formulas!$J$1:'Formulas'!$J$18)&lt;19)*(Formulas!$J$1:'Formulas'!$J$18&lt;&gt;""))</f>
-        <v>45383</v>
+        <v>45413</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C2" s="4">
-        <v>45384</v>
+        <v>45414</v>
       </c>
       <c r="D2" s="5">
         <f t="shared" ref="D2:D31" si="2">IF($C2="","",WEEKDAY($C2)-1)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="4">
-        <v>45384</v>
+        <v>45414</v>
       </c>
       <c r="G2" s="5">
         <f t="shared" ref="G2:G31" si="3">IF($F2="","",WEEKDAY($F2)-1)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H2" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="18">
-        <v>45384</v>
+        <v>45414</v>
       </c>
       <c r="K2" s="16" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="5" t="str">
@@ -10693,38 +10707,38 @@
         <v>2</v>
       </c>
       <c r="P2" s="23" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="Q2" s="24">
-        <v>45384</v>
+        <v>45414</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C3" s="4">
-        <v>45385</v>
+        <v>45415</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="4">
-        <v>45385</v>
+        <v>45415</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H3" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="18">
-        <v>45385</v>
+        <v>45415</v>
       </c>
       <c r="K3" s="16" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="5" t="str">
@@ -10735,38 +10749,38 @@
         <v>3</v>
       </c>
       <c r="P3" s="23" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="Q3" s="24">
-        <v>45385</v>
+        <v>45415</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C4" s="4">
-        <v>45386</v>
+        <v>45416</v>
       </c>
       <c r="D4" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="4">
-        <v>45386</v>
+        <v>45416</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H4" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="18">
-        <v>45386</v>
+        <v>45416</v>
       </c>
       <c r="K4" s="16" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="5" t="str">
@@ -10777,38 +10791,38 @@
         <v>4</v>
       </c>
       <c r="P4" s="23" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="Q4" s="24">
-        <v>45386</v>
+        <v>45416</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C5" s="4">
-        <v>45387</v>
+        <v>45417</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="4">
-        <v>45387</v>
+        <v>45418</v>
       </c>
       <c r="G5" s="5">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H5" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="18">
-        <v>45387</v>
+        <v>45418</v>
       </c>
       <c r="K5" s="16" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="5" t="str">
@@ -10819,38 +10833,38 @@
         <v>5</v>
       </c>
       <c r="P5" s="23" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="Q5" s="24">
-        <v>45387</v>
+        <v>45418</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C6" s="4">
-        <v>45388</v>
+        <v>45418</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="4">
-        <v>45388</v>
+        <v>45419</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H6" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="18">
-        <v>45388</v>
+        <v>45419</v>
       </c>
       <c r="K6" s="16" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="5" t="str">
@@ -10861,474 +10875,474 @@
         <v>6</v>
       </c>
       <c r="P6" s="23" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="Q6" s="24">
-        <v>45388</v>
+        <v>45419</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C7" s="4">
-        <v>45389</v>
+        <v>45419</v>
       </c>
       <c r="D7" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="4">
-        <v>45390</v>
+        <v>45420</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H7" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="18">
-        <v>45390</v>
+        <v>45420</v>
       </c>
       <c r="K7" s="16" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="P7" s="23" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="Q7" s="24">
-        <v>45390</v>
+        <v>45420</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C8" s="4">
-        <v>45390</v>
+        <v>45420</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="4">
-        <v>45391</v>
+        <v>45421</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H8" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="18">
-        <v>45391</v>
+        <v>45421</v>
       </c>
       <c r="K8" s="16" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="15"/>
       <c r="N8" s="17"/>
       <c r="P8" s="23" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="Q8" s="24">
-        <v>45391</v>
+        <v>45421</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C9" s="4">
-        <v>45391</v>
+        <v>45421</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="4">
-        <v>45392</v>
+        <v>45422</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H9" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="18">
-        <v>45392</v>
+        <v>45422</v>
       </c>
       <c r="K9" s="16" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="P9" s="23" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="Q9" s="24">
-        <v>45392</v>
+        <v>45422</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C10" s="4">
-        <v>45392</v>
+        <v>45422</v>
       </c>
       <c r="D10" s="5">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="4">
-        <v>45393</v>
+        <v>45423</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H10" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="18">
-        <v>45393</v>
+        <v>45423</v>
       </c>
       <c r="K10" s="16" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="20"/>
       <c r="P10" s="23" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="Q10" s="24">
-        <v>45393</v>
+        <v>45423</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C11" s="4">
-        <v>45393</v>
+        <v>45423</v>
       </c>
       <c r="D11" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="4">
-        <v>45394</v>
+        <v>45425</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H11" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="18">
-        <v>45394</v>
+        <v>45425</v>
       </c>
       <c r="K11" s="16" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="P11" s="23" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="Q11" s="24">
-        <v>45394</v>
+        <v>45425</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C12" s="4">
-        <v>45394</v>
+        <v>45424</v>
       </c>
       <c r="D12" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="4">
-        <v>45395</v>
+        <v>45426</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H12" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="18">
-        <v>45395</v>
+        <v>45426</v>
       </c>
       <c r="K12" s="16" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="P12" s="23" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="Q12" s="24">
-        <v>45395</v>
+        <v>45426</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C13" s="4">
-        <v>45395</v>
+        <v>45425</v>
       </c>
       <c r="D13" s="5">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="4">
-        <v>45397</v>
+        <v>45427</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H13" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="18">
-        <v>45397</v>
+        <v>45427</v>
       </c>
       <c r="K13" s="16" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="20"/>
       <c r="N13" s="6"/>
       <c r="P13" s="23" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="Q13" s="24">
-        <v>45397</v>
+        <v>45427</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C14" s="4">
-        <v>45396</v>
+        <v>45426</v>
       </c>
       <c r="D14" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="4">
-        <v>45398</v>
+        <v>45428</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H14" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="18">
-        <v>45398</v>
+        <v>45428</v>
       </c>
       <c r="K14" s="16" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="L14" s="6"/>
       <c r="M14" s="20"/>
       <c r="N14" s="20"/>
       <c r="P14" s="23" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="Q14" s="24">
-        <v>45398</v>
+        <v>45428</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C15" s="4">
-        <v>45397</v>
+        <v>45427</v>
       </c>
       <c r="D15" s="5">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="4">
-        <v>45399</v>
+        <v>45429</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H15" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="18">
-        <v>45399</v>
+        <v>45429</v>
       </c>
       <c r="K15" s="16" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="P15" s="23" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="Q15" s="24">
-        <v>45399</v>
+        <v>45429</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C16" s="4">
-        <v>45398</v>
+        <v>45428</v>
       </c>
       <c r="D16" s="5">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="4">
-        <v>45400</v>
+        <v>45430</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H16" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="18">
-        <v>45400</v>
+        <v>45430</v>
       </c>
       <c r="K16" s="16" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="P16" s="23" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="Q16" s="24">
-        <v>45400</v>
+        <v>45430</v>
       </c>
     </row>
     <row r="17" spans="3:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C17" s="4">
-        <v>45399</v>
+        <v>45429</v>
       </c>
       <c r="D17" s="5">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="4">
-        <v>45401</v>
+        <v>45432</v>
       </c>
       <c r="G17" s="5">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="18">
-        <v>45401</v>
+        <v>45432</v>
       </c>
       <c r="K17" s="16" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="L17" s="6"/>
       <c r="M17" s="20"/>
       <c r="N17" s="6"/>
       <c r="P17" s="23" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="Q17" s="24">
-        <v>45401</v>
+        <v>45432</v>
       </c>
     </row>
     <row r="18" spans="3:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C18" s="4">
-        <v>45400</v>
+        <v>45430</v>
       </c>
       <c r="D18" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="4">
-        <v>45402</v>
+        <v>45433</v>
       </c>
       <c r="G18" s="5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H18" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="18">
-        <v>45402</v>
+        <v>45433</v>
       </c>
       <c r="K18" s="16" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="L18" s="6"/>
       <c r="N18" s="6"/>
       <c r="P18" s="23" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="Q18" s="24">
-        <v>45402</v>
+        <v>45433</v>
       </c>
     </row>
     <row r="19" spans="3:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C19" s="4">
-        <v>45401</v>
+        <v>45431</v>
       </c>
       <c r="D19" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="4">
-        <v>45404</v>
+        <v>45434</v>
       </c>
       <c r="G19" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H19" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="21"/>
@@ -11339,309 +11353,311 @@
     </row>
     <row r="20" spans="3:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C20" s="4">
-        <v>45402</v>
+        <v>45432</v>
       </c>
       <c r="D20" s="5">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="4">
-        <v>45405</v>
+        <v>45435</v>
       </c>
       <c r="G20" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H20" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="18" cm="1">
-        <f t="array" ref="J20:J27">IF(ISBLANK($F$19),"",IF(ISBLANK($F$24), _xlfn._xlws.FILTER($F$1:$F$31, (ROW($F$1:$F$31)&gt;COUNT($F$1:$F$31)-5)*($F$1:$F$31&lt;&gt;"")),_xlfn._xlws.FILTER($F$1:$F$31, (ROW($F$1:$F$31)&gt;=19)*($F$1:$F$31&lt;&gt;""))))</f>
-        <v>45404</v>
+        <f t="array" ref="J20:J28">IF(ISBLANK($F$19),"",IF(ISBLANK($F$24), _xlfn._xlws.FILTER($F$1:$F$31, (ROW($F$1:$F$31)&gt;COUNT($F$1:$F$31)-5)*($F$1:$F$31&lt;&gt;"")),_xlfn._xlws.FILTER($F$1:$F$31, (ROW($F$1:$F$31)&gt;=19)*($F$1:$F$31&lt;&gt;""))))</f>
+        <v>45434</v>
       </c>
       <c r="K20" s="16" t="str" cm="1">
-        <f t="array" ref="K20:K27">IF(ISBLANK($F$19),"",IF(ISBLANK($F$24), _xlfn._xlws.FILTER($H$1:$H$31, (ROW($F$1:$F$31)&gt;COUNT($F$1:$F$31)-5)*($F$1:$F$31&lt;&gt;"")),_xlfn._xlws.FILTER($H$1:$H$31, (ROW($F$1:$F$31)&gt;=19)*($F$1:$F$31&lt;&gt;""))))</f>
-        <v>星期一</v>
+        <f t="array" ref="K20:K28">IF(ISBLANK($F$19),"",IF(ISBLANK($F$24), _xlfn._xlws.FILTER($H$1:$H$31, (ROW($F$1:$F$31)&gt;COUNT($F$1:$F$31)-5)*($F$1:$F$31&lt;&gt;"")),_xlfn._xlws.FILTER($H$1:$H$31, (ROW($F$1:$F$31)&gt;=19)*($F$1:$F$31&lt;&gt;""))))</f>
+        <v>星期三</v>
       </c>
       <c r="L20" s="6"/>
       <c r="M20" s="15"/>
       <c r="N20" s="6"/>
       <c r="P20" s="25" t="str" cm="1">
-        <f t="array" ref="P20:P27">IFERROR(_xlfn._xlws.FILTER(Formulas!$K$20:'Formulas'!$K$31, (ROW(Formulas!$K$20:'Formulas'!$K$31)&gt;19)*(Formulas!$K$20:'Formulas'!$K$31&lt;&gt;"")), "")</f>
-        <v>星期一</v>
+        <f t="array" ref="P20:P28">IFERROR(_xlfn._xlws.FILTER(Formulas!$K$20:'Formulas'!$K$31, (ROW(Formulas!$K$20:'Formulas'!$K$31)&gt;19)*(Formulas!$K$20:'Formulas'!$K$31&lt;&gt;"")), "")</f>
+        <v>星期三</v>
       </c>
       <c r="Q20" s="26" cm="1">
-        <f t="array" ref="Q20:Q27">IFERROR(_xlfn._xlws.FILTER(Formulas!$J$20:'Formulas'!$J$31, (ROW(Formulas!$J$20:'Formulas'!$J$31)&gt;19)*(Formulas!$J$20:'Formulas'!$J$31&lt;&gt;"")), "")</f>
-        <v>45404</v>
+        <f t="array" ref="Q20:Q28">IFERROR(_xlfn._xlws.FILTER(Formulas!$J$20:'Formulas'!$J$31, (ROW(Formulas!$J$20:'Formulas'!$J$31)&gt;19)*(Formulas!$J$20:'Formulas'!$J$31&lt;&gt;"")), "")</f>
+        <v>45434</v>
       </c>
     </row>
     <row r="21" spans="3:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C21" s="4">
-        <v>45403</v>
+        <v>45433</v>
       </c>
       <c r="D21" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="4">
-        <v>45406</v>
+        <v>45436</v>
       </c>
       <c r="G21" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H21" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="18">
-        <v>45405</v>
+        <v>45435</v>
       </c>
       <c r="K21" s="16" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="P21" s="23" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="Q21" s="24">
-        <v>45405</v>
+        <v>45435</v>
       </c>
     </row>
     <row r="22" spans="3:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C22" s="4">
-        <v>45404</v>
+        <v>45434</v>
       </c>
       <c r="D22" s="5">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="4">
-        <v>45407</v>
+        <v>45437</v>
       </c>
       <c r="G22" s="5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H22" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="18">
-        <v>45406</v>
+        <v>45436</v>
       </c>
       <c r="K22" s="16" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="P22" s="23" t="str">
-        <v>星期三</v>
+        <v>星期五</v>
       </c>
       <c r="Q22" s="24">
-        <v>45406</v>
+        <v>45436</v>
       </c>
     </row>
     <row r="23" spans="3:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C23" s="4">
-        <v>45405</v>
+        <v>45435</v>
       </c>
       <c r="D23" s="5">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="4">
-        <v>45408</v>
+        <v>45439</v>
       </c>
       <c r="G23" s="5">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H23" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="18">
-        <v>45407</v>
+        <v>45437</v>
       </c>
       <c r="K23" s="16" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="P23" s="23" t="str">
-        <v>星期四</v>
+        <v>星期六</v>
       </c>
       <c r="Q23" s="24">
-        <v>45407</v>
+        <v>45437</v>
       </c>
     </row>
     <row r="24" spans="3:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C24" s="4">
-        <v>45406</v>
+        <v>45436</v>
       </c>
       <c r="D24" s="5">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="4">
-        <v>45409</v>
+        <v>45440</v>
       </c>
       <c r="G24" s="5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H24" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="18">
-        <v>45408</v>
+        <v>45439</v>
       </c>
       <c r="K24" s="16" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="P24" s="23" t="str">
-        <v>星期五</v>
+        <v>星期一</v>
       </c>
       <c r="Q24" s="24">
-        <v>45408</v>
+        <v>45439</v>
       </c>
     </row>
     <row r="25" spans="3:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="4">
-        <v>45407</v>
+        <v>45437</v>
       </c>
       <c r="D25" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="4">
-        <v>45411</v>
+        <v>45441</v>
       </c>
       <c r="G25" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H25" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="18">
-        <v>45409</v>
+        <v>45440</v>
       </c>
       <c r="K25" s="16" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="P25" s="23" t="str">
-        <v>星期六</v>
+        <v>星期二</v>
       </c>
       <c r="Q25" s="24">
-        <v>45409</v>
+        <v>45440</v>
       </c>
     </row>
     <row r="26" spans="3:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C26" s="4">
-        <v>45408</v>
+        <v>45438</v>
       </c>
       <c r="D26" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="4">
-        <v>45412</v>
+        <v>45442</v>
       </c>
       <c r="G26" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H26" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="18">
-        <v>45411</v>
+        <v>45441</v>
       </c>
       <c r="K26" s="16" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="P26" s="23" t="str">
-        <v>星期一</v>
+        <v>星期三</v>
       </c>
       <c r="Q26" s="24">
-        <v>45411</v>
+        <v>45441</v>
       </c>
     </row>
     <row r="27" spans="3:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C27" s="4">
-        <v>45409</v>
+        <v>45439</v>
       </c>
       <c r="D27" s="5">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E27" s="6"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="5" t="str">
+      <c r="F27" s="4">
+        <v>45443</v>
+      </c>
+      <c r="G27" s="5">
         <f t="shared" si="3"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="H27" s="5" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>星期五</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="18">
-        <v>45412</v>
+        <v>45442</v>
       </c>
       <c r="K27" s="16" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="P27" s="23" t="str">
-        <v>星期二</v>
+        <v>星期四</v>
       </c>
       <c r="Q27" s="24">
-        <v>45412</v>
+        <v>45442</v>
       </c>
     </row>
     <row r="28" spans="3:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C28" s="4">
-        <v>45410</v>
+        <v>45440</v>
       </c>
       <c r="D28" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="4"/>
@@ -11654,19 +11670,29 @@
         <v/>
       </c>
       <c r="I28" s="6"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="16"/>
+      <c r="J28" s="18">
+        <v>45443</v>
+      </c>
+      <c r="K28" s="16" t="str">
+        <v>星期五</v>
+      </c>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
+      <c r="P28" s="23" t="str">
+        <v>星期五</v>
+      </c>
+      <c r="Q28" s="24">
+        <v>45443</v>
+      </c>
     </row>
     <row r="29" spans="3:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C29" s="4">
-        <v>45411</v>
+        <v>45441</v>
       </c>
       <c r="D29" s="5">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="4"/>
@@ -11687,11 +11713,11 @@
     </row>
     <row r="30" spans="3:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C30" s="4">
-        <v>45412</v>
+        <v>45442</v>
       </c>
       <c r="D30" s="5">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="4"/>
@@ -11711,10 +11737,12 @@
       <c r="N30" s="6"/>
     </row>
     <row r="31" spans="3:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="4"/>
-      <c r="D31" s="5" t="str">
+      <c r="C31" s="4">
+        <v>45443</v>
+      </c>
+      <c r="D31" s="5">
         <f t="shared" si="2"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="4"/>

</xml_diff>

<commit_message>
Excel logic (v1 in prog)
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\TimeSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AE0892-3E5A-4C45-B0FB-5D9D1FDADF5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70E3BA88-FDE4-46F1-96E4-BBD8A22B675D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="1900" windowWidth="13330" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">AUTHORIZED DAYS:    </t>
   </si>
@@ -85,9 +85,6 @@
     <t>Day</t>
   </si>
   <si>
-    <t>MON TUE WED THU FRI SAT</t>
-  </si>
-  <si>
     <t>EFFECTIVE: 01/01/2024 TO 01/31/2025</t>
   </si>
   <si>
@@ -126,13 +123,19 @@
   <si>
     <t xml:space="preserve">DIA CODE: </t>
   </si>
+  <si>
+    <t>Yo</t>
+  </si>
+  <si>
+    <t>MON TUE WED</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -247,7 +250,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -257,14 +260,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -555,7 +558,7 @@
   <dimension ref="A1:H964"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -569,7 +572,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -581,7 +584,7 @@
     </row>
     <row r="2" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -603,25 +606,25 @@
     </row>
     <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -633,15 +636,15 @@
     </row>
     <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -649,14 +652,14 @@
     </row>
     <row r="7" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -669,7 +672,7 @@
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="17" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="12"/>
@@ -736,7 +739,9 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8"/>
+      <c r="A12" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="B12" s="7"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>

</xml_diff>

<commit_message>
get weekdays of month
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\TimeSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70E3BA88-FDE4-46F1-96E4-BBD8A22B675D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF438DF2-6182-4F1E-8E09-52270539A14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">AUTHORIZED DAYS:    </t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t xml:space="preserve">DIA CODE: </t>
-  </si>
-  <si>
-    <t>Yo</t>
   </si>
   <si>
     <t>MON TUE WED</t>
@@ -672,7 +669,7 @@
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="12"/>
@@ -739,9 +736,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="A12" s="8"/>
       <c r="B12" s="7"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>

</xml_diff>

<commit_message>
Write dates to excel
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\TimeSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF438DF2-6182-4F1E-8E09-52270539A14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{083FCB29-8944-4F35-9A58-FE1398FEBBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t xml:space="preserve">AUTHORIZED DAYS:    </t>
   </si>
@@ -125,6 +125,15 @@
   </si>
   <si>
     <t>MON TUE WED</t>
+  </si>
+  <si>
+    <t>星期一</t>
+  </si>
+  <si>
+    <t>星期二</t>
+  </si>
+  <si>
+    <t>星期三</t>
   </si>
 </sst>
 </file>
@@ -736,8 +745,12 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="7">
+        <v>45355</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -746,48 +759,92 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="8"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="7">
+        <v>45356</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="8"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="7">
+        <v>45357</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="8"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="7">
+        <v>45362</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="8"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="7">
+        <v>45363</v>
+      </c>
     </row>
     <row r="17" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="7">
+        <v>45364</v>
+      </c>
     </row>
     <row r="18" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="8"/>
-      <c r="B18" s="7"/>
+      <c r="A18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="7">
+        <v>45369</v>
+      </c>
     </row>
     <row r="19" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="8"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="7">
+        <v>45370</v>
+      </c>
     </row>
     <row r="20" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="8"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="7">
+        <v>45371</v>
+      </c>
     </row>
     <row r="21" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="8"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="7">
+        <v>45376</v>
+      </c>
     </row>
     <row r="22" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="7">
+        <v>45377</v>
+      </c>
     </row>
     <row r="23" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="7">
+        <v>45378</v>
+      </c>
     </row>
     <row r="24" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8"/>

</xml_diff>